<commit_message>
opdateret til også at kigge efter indsatspakker
</commit_message>
<xml_diff>
--- a/Indsatser.xlsx
+++ b/Indsatser.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\RPA\Leverancer\Automatisk filtrering af Medcoms for Sambovagten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakkw\source\automatisk-filtrering-af-medcoms-for-sambovagten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D17B2A21-3A2D-4371-9F70-9FCDB5809DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06794392-F964-48C6-B754-C4F2D66F6BB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Liste" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="90">
   <si>
     <t>Navn</t>
   </si>
@@ -294,6 +294,18 @@
   </si>
   <si>
     <t>Afløsning i hjemmet</t>
+  </si>
+  <si>
+    <t>Dag - opstartsindsatser SEL § 83 a</t>
+  </si>
+  <si>
+    <t>Aften - opstartsindsatser SEL § 83 a</t>
+  </si>
+  <si>
+    <t>Dag -- Terminalpakke Servicelov</t>
+  </si>
+  <si>
+    <t>Aften -- Terminalpakke Servicelov</t>
   </si>
 </sst>
 </file>
@@ -665,19 +677,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B83"/>
+  <dimension ref="A1:B87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="76.26953125" customWidth="1"/>
-    <col min="2" max="2" width="29.26953125" customWidth="1"/>
+    <col min="1" max="1" width="76.28515625" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -685,7 +697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -693,7 +705,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -701,7 +713,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -709,7 +721,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -717,7 +729,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -725,7 +737,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -733,7 +745,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -741,7 +753,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -749,7 +761,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -757,7 +769,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -765,7 +777,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -773,7 +785,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -781,7 +793,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -789,7 +801,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -797,7 +809,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -805,7 +817,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -813,7 +825,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -821,7 +833,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -829,7 +841,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -837,7 +849,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -845,7 +857,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -853,7 +865,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -861,7 +873,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -869,7 +881,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -877,7 +889,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -885,7 +897,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -893,7 +905,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -901,7 +913,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -909,7 +921,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -917,7 +929,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -925,7 +937,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -933,7 +945,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -941,7 +953,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -949,7 +961,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -957,7 +969,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -965,7 +977,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -973,7 +985,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -981,7 +993,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -989,7 +1001,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -997,7 +1009,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -1005,7 +1017,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -1013,7 +1025,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -1021,7 +1033,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -1029,7 +1041,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -1037,7 +1049,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -1045,7 +1057,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -1053,7 +1065,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -1061,7 +1073,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -1069,7 +1081,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>52</v>
       </c>
@@ -1077,169 +1089,189 @@
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>